<commit_message>
updated charts, GetFile method
</commit_message>
<xml_diff>
--- a/LGEBills.xlsx
+++ b/LGEBills.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CodeLouisville\repos\CLP-LGEBills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0745B0A5-7EDA-4B6A-9CED-B56C3E678573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7227172D-7C5E-4C17-9E0F-58F52F16231B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,10 +346,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -1105,16 +1105,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bill Data'!$L$2:$L$253</c:f>
+              <c:f>'Bill Data'!$L$2:$L$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.0000</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>5.6970227670753069E-2</c:v>
                 </c:pt>
@@ -1870,6 +1873,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>0.11794612794612795</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.11223577235772357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1917,10 +1923,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -2676,16 +2682,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bill Data'!$S$2:$S$253</c:f>
+              <c:f>'Bill Data'!$S$2:$S$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.0000</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>0.68999999999999984</c:v>
                 </c:pt>
@@ -3441,6 +3450,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>1.4424999999999999</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1.5899999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3645,10 +3657,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -4404,16 +4416,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$R$2:$R$253</c:f>
+              <c:f>'Bill Data'!$R$2:$R$254</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -5169,6 +5184,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5221,10 +5239,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -5980,16 +5998,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$N$2:$N$253</c:f>
+              <c:f>'Bill Data'!$N$2:$N$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>8.6999999999999993</c:v>
                 </c:pt>
@@ -6745,6 +6766,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>31.69</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>29.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6799,10 +6823,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -7558,16 +7582,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$F$2:$F$253</c:f>
+              <c:f>'Bill Data'!$F$2:$F$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>43.7</c:v>
                 </c:pt>
@@ -8323,6 +8350,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>150.73000000000002</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>125.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8524,10 +8554,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -9283,16 +9313,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$K$2:$K$253</c:f>
+              <c:f>'Bill Data'!$K$2:$K$254</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>571</c:v>
                 </c:pt>
@@ -10048,6 +10081,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10110,10 +10146,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -10869,16 +10905,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$G$2:$G$253</c:f>
+              <c:f>'Bill Data'!$G$2:$G$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>35</c:v>
                 </c:pt>
@@ -11634,6 +11673,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>119.04</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>96.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11688,10 +11730,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -12447,16 +12489,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$F$2:$F$253</c:f>
+              <c:f>'Bill Data'!$F$2:$F$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>43.7</c:v>
                 </c:pt>
@@ -13212,6 +13257,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>150.73000000000002</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>125.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13389,10 +13437,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -14148,16 +14196,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bill Data'!$N$2:$N$253</c:f>
+              <c:f>'Bill Data'!$N$2:$N$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>8.6999999999999993</c:v>
                 </c:pt>
@@ -14913,6 +14964,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>31.69</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>29.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14946,10 +15000,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Bill Data'!$A$2:$A$253</c:f>
+              <c:f>'Bill Data'!$A$2:$A$254</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>37175</c:v>
                 </c:pt>
@@ -15705,16 +15759,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bill Data'!$G$2:$G$253</c:f>
+              <c:f>'Bill Data'!$G$2:$G$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>35</c:v>
                 </c:pt>
@@ -16470,6 +16527,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>119.04</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>96.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16643,7 +16703,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{56609F23-C0E0-4F98-AE9D-4C80EBB288B0}</c15:txfldGUID>
+                      <c15:txfldGUID>{EB24038B-0017-4857-A168-BDBD8FC05A06}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$2</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16684,7 +16744,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{248F164E-DD4A-4B6B-80DF-0C2A41428723}</c15:txfldGUID>
+                      <c15:txfldGUID>{77EC0EF7-AD85-4C7D-859B-FE716E48878D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$3</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16725,7 +16785,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2634E471-2AA6-4A79-A342-6432FD113AF7}</c15:txfldGUID>
+                      <c15:txfldGUID>{1E46530D-44AD-4DF6-9C98-FA9DD8E9D556}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$4</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16766,7 +16826,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{516EE307-5608-4044-A282-E0D8DC3DEC11}</c15:txfldGUID>
+                      <c15:txfldGUID>{5BF8EF69-89DC-4210-95BB-F05EB9F62187}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16807,7 +16867,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{673BB310-5A67-44AE-AA8A-3392C37972C7}</c15:txfldGUID>
+                      <c15:txfldGUID>{0EBFE4A0-87CD-45E1-B425-C548BA06864C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$6</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16848,7 +16908,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BB42202F-3A19-4A6B-8871-575387AF4087}</c15:txfldGUID>
+                      <c15:txfldGUID>{D107B007-0680-4A2B-B986-53BD95E7C1A0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$7</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16889,7 +16949,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E85783DD-2F8F-466E-99AB-67811B607521}</c15:txfldGUID>
+                      <c15:txfldGUID>{1A987210-0F0B-4540-856A-335E8971510E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$8</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16930,7 +16990,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7EE4EF64-A2AD-4D75-AC1A-CAA6918E0619}</c15:txfldGUID>
+                      <c15:txfldGUID>{844FF2FB-0A7D-4C1E-B7AA-863CB9297C4F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$9</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -16971,7 +17031,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5B120BFE-FAB6-454A-81AB-B354A1A0BF7B}</c15:txfldGUID>
+                      <c15:txfldGUID>{E54E66B7-A81E-4EB6-8592-126EE60921F6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$10</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17012,7 +17072,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5723EBEB-E337-48C4-BAAC-2C3EBE9C4456}</c15:txfldGUID>
+                      <c15:txfldGUID>{204BF0C2-5BF4-49C8-B6C1-3FF39B650A59}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$11</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17053,7 +17113,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8AEFE42A-E8BE-483F-9C3F-41E9DE95A232}</c15:txfldGUID>
+                      <c15:txfldGUID>{67EAA243-1EDC-4EE3-9126-A6F0437427F6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$12</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17094,7 +17154,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2F322658-A600-4672-991C-06E5A588BC16}</c15:txfldGUID>
+                      <c15:txfldGUID>{B9D40AC0-C10F-487D-B3D9-6F286EB1A8B2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$13</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17135,7 +17195,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5CF7FABD-6E2A-475A-8FCC-C9A4F8F9ECA6}</c15:txfldGUID>
+                      <c15:txfldGUID>{6D391C01-2E0C-4579-A01F-2D4658A08D28}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$14</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17176,7 +17236,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E220D54A-2D7D-4CE7-89EB-25F4C939A858}</c15:txfldGUID>
+                      <c15:txfldGUID>{CA4953EC-3256-4D2B-833E-FB57B3828B3A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$15</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17217,7 +17277,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6E2A267C-9904-4D93-8612-9AA28AF3D447}</c15:txfldGUID>
+                      <c15:txfldGUID>{DBA980DB-328C-4F9D-80F0-AED6410FE583}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$16</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17258,7 +17318,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{41F0EDD2-935C-4029-9368-389C1894EC00}</c15:txfldGUID>
+                      <c15:txfldGUID>{9BEB8DF1-52E7-4795-AB13-5F043025701C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$17</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17299,7 +17359,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0D7357BB-B4E3-4FCD-8AB0-61675CD88C67}</c15:txfldGUID>
+                      <c15:txfldGUID>{C4622198-D4A1-4779-A716-B3C89E73466A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$18</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17340,7 +17400,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3A791C67-986C-4433-B107-D7AE3EC8107F}</c15:txfldGUID>
+                      <c15:txfldGUID>{D7B00876-710C-4C6C-8165-FB47932193F9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$19</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17381,7 +17441,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A2B24EA5-C021-44F2-BA61-32ACF368D61D}</c15:txfldGUID>
+                      <c15:txfldGUID>{2DECC638-217C-4D82-A487-7A0322CBE713}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$20</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17422,7 +17482,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{63350B1D-9C74-470E-BFA2-10027E44E37D}</c15:txfldGUID>
+                      <c15:txfldGUID>{404FBED9-E71E-477D-9CB3-D5913FC6D0E1}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$21</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17463,7 +17523,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F4E21618-BA52-481D-B1DC-CEC410C0A61C}</c15:txfldGUID>
+                      <c15:txfldGUID>{17A3488C-8CA6-4225-853C-091323E21B0E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$22</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17504,7 +17564,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BBD1B233-EC46-43E8-A1D2-1F873C640E58}</c15:txfldGUID>
+                      <c15:txfldGUID>{FD217B27-2E79-425E-B556-8310CDE1A4F0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$23</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17545,7 +17605,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2DF47815-49ED-4168-9BD8-FD4678F42B8A}</c15:txfldGUID>
+                      <c15:txfldGUID>{C021DC0A-5EDA-4254-8D12-8763F0E171FB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$24</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17586,7 +17646,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{174CC14E-2D64-4655-8B44-F18A063A654D}</c15:txfldGUID>
+                      <c15:txfldGUID>{2062E6BC-ADC8-4EFB-852E-7FFE31D62C09}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$25</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17627,7 +17687,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DC283BD2-51C4-4F4C-8759-F50422533931}</c15:txfldGUID>
+                      <c15:txfldGUID>{AB3C812E-66EB-4227-B7A4-ACBB98BE9AE2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$26</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17668,7 +17728,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4A8AF092-0F08-4A24-95F8-F4E0765E39F8}</c15:txfldGUID>
+                      <c15:txfldGUID>{3315C56F-BA17-497B-88EC-C272D79A1AD9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$27</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17709,7 +17769,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{74E7A6E1-49A2-4A37-AC0B-74CB020E2CBF}</c15:txfldGUID>
+                      <c15:txfldGUID>{9D901364-7008-48F1-944A-7A022978D779}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$28</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17750,7 +17810,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{84FCB66C-4334-4304-B72B-DF19731B9F44}</c15:txfldGUID>
+                      <c15:txfldGUID>{5D076F97-6419-4791-80B2-4561949FA16D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$29</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17791,7 +17851,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B8D04B52-75A0-44D8-A30B-0D41E7CA9E75}</c15:txfldGUID>
+                      <c15:txfldGUID>{D5CD7432-46CE-4A75-8923-3771C7022A4C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$30</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17832,7 +17892,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A12F3DF6-61F6-4BAD-82AE-564E54E6FBE8}</c15:txfldGUID>
+                      <c15:txfldGUID>{5EB03A86-2E0F-4DEF-862B-A31D6B2071F9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$31</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17873,7 +17933,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{414D5360-C769-411C-945F-EA46450C6C1A}</c15:txfldGUID>
+                      <c15:txfldGUID>{D943F731-08C4-4281-9796-29CE70B39332}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$32</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17914,7 +17974,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F89A84A7-E681-4BAC-BA08-DF48DB70E598}</c15:txfldGUID>
+                      <c15:txfldGUID>{07E92453-EA01-4EC0-85A7-57D1B48D1A7A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$33</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17955,7 +18015,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CD8942B2-BF21-473E-88DF-9F6FE4FDC1A1}</c15:txfldGUID>
+                      <c15:txfldGUID>{7BDA6B2D-349A-4E99-8A1A-EF5A8D2C21AA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$34</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -17996,7 +18056,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{21025176-AE35-4BEB-BBA8-0978BCE6C8C4}</c15:txfldGUID>
+                      <c15:txfldGUID>{2150BCE9-70FE-45EF-8DA4-9C614D54BFBF}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$35</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18037,7 +18097,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C4DFEAF9-FDF5-42FE-82B1-1BED602B4DD7}</c15:txfldGUID>
+                      <c15:txfldGUID>{845C8A70-53CD-4D8E-B33C-D7507B7B8AB0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$36</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18078,7 +18138,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6EB41841-2184-4299-88FF-720AA5AFBDFC}</c15:txfldGUID>
+                      <c15:txfldGUID>{2A36E5D3-4260-4AC6-B0B5-3EF8ACC217A4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$37</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18119,7 +18179,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E65588A3-BF87-41DF-8C89-43FA20AB6ABB}</c15:txfldGUID>
+                      <c15:txfldGUID>{7C225A74-042A-490A-B283-E1B9F7B1D7C0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$38</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18160,7 +18220,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DACD6926-6308-4C50-B417-0CAB6AA7FE39}</c15:txfldGUID>
+                      <c15:txfldGUID>{B3C61EC5-425E-4F23-9B59-04CAE86374E4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$39</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18201,7 +18261,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{24886E5A-F1DE-41A6-B2A2-823A8D7CBD5C}</c15:txfldGUID>
+                      <c15:txfldGUID>{F87F3A4B-895A-43FE-B3AA-E127095E2C51}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$40</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18242,7 +18302,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FF199E21-DAA6-4182-B7DF-3FD92AC2C0FC}</c15:txfldGUID>
+                      <c15:txfldGUID>{74F1D83E-E5C4-40FB-87B5-FE7A8AB63BA0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$41</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18283,7 +18343,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1B231FF9-EE07-4506-83AF-0D81581870C9}</c15:txfldGUID>
+                      <c15:txfldGUID>{ED421B84-1FBB-402F-9C98-B27D8A4296B1}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$42</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18324,7 +18384,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{53D40540-3123-479E-9E38-39E257F3C916}</c15:txfldGUID>
+                      <c15:txfldGUID>{7C43EB47-B9A5-4461-AF8B-4858DFB20C06}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$43</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18365,7 +18425,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{064DCA70-5667-4F64-BA50-2B5DFCFC97B8}</c15:txfldGUID>
+                      <c15:txfldGUID>{5FB33D4E-18DD-4BCA-85E9-6BE8EB38ECEF}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$44</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18406,7 +18466,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{13A15D00-76C2-4299-9C6E-234BEF3FA4C1}</c15:txfldGUID>
+                      <c15:txfldGUID>{776583BF-585A-4014-BFA1-7C6490121F91}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$45</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18447,7 +18507,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8A7664E1-8169-4115-95D0-78D84B330F49}</c15:txfldGUID>
+                      <c15:txfldGUID>{B51433E4-E008-4B7B-AFFA-D3426A84F773}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$46</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18488,7 +18548,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F1B36ECD-3A37-41EA-9068-B87AB0E0B433}</c15:txfldGUID>
+                      <c15:txfldGUID>{A576B116-DF8C-457B-A156-06C179EF7DFF}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$47</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18529,7 +18589,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D85D97F7-2966-4899-AC38-6E5CE81978EF}</c15:txfldGUID>
+                      <c15:txfldGUID>{8304BECF-237D-4870-87DE-FFE2CD0A0CCF}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$48</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18570,7 +18630,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B163D1A9-494B-4565-8C88-A92E5FB26401}</c15:txfldGUID>
+                      <c15:txfldGUID>{C3210D79-B6D4-454A-988A-0BF85D04D0E9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$49</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18611,7 +18671,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2A8D7A9C-3452-4B00-9A35-FAC906841928}</c15:txfldGUID>
+                      <c15:txfldGUID>{5F6B85AD-F703-4E35-8DDD-9EBC05128B6F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$50</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18652,7 +18712,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{16A62FBA-E611-47D0-8DA0-1E5794804073}</c15:txfldGUID>
+                      <c15:txfldGUID>{914C98E2-25B0-468C-9A2C-4E74CD7F829C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$51</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18693,7 +18753,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D6E4FA6A-0854-492A-B617-7CC085EBD7DB}</c15:txfldGUID>
+                      <c15:txfldGUID>{8920D8E6-342B-4A7B-A294-BD9F84230556}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$52</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18734,7 +18794,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{16A23082-8949-4A81-9B56-DA56CCD095CA}</c15:txfldGUID>
+                      <c15:txfldGUID>{BACAF2F1-1AD3-4337-827C-D49F4A95E660}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$53</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18775,7 +18835,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0BBFB43F-E964-4FD6-BF71-1E6A5526C4A8}</c15:txfldGUID>
+                      <c15:txfldGUID>{7E56A606-DAE0-42D9-969F-5E33C4135FDD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$54</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18816,7 +18876,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3B23B227-9563-465D-AB76-863A494D137D}</c15:txfldGUID>
+                      <c15:txfldGUID>{47824F53-F266-4646-844D-9AE5EF40FFF3}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$55</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18857,7 +18917,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7DCB174C-0B8E-4485-98EB-914577D3C7E9}</c15:txfldGUID>
+                      <c15:txfldGUID>{0E3E4EDB-0C1B-465C-A38D-2883D906B420}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$56</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18898,7 +18958,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0D712E5E-C291-4A09-A8D4-E90331279C53}</c15:txfldGUID>
+                      <c15:txfldGUID>{5B3C541D-1E28-43EA-827D-F96E5054B8A7}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$57</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18939,7 +18999,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BC90DB71-6EC9-41C2-B8AE-38CD69589BE4}</c15:txfldGUID>
+                      <c15:txfldGUID>{B83EDC20-0063-4D47-B2E7-7CAB5252589B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$58</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -18980,7 +19040,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E04C9511-3A3E-46B0-8088-4A43F382757C}</c15:txfldGUID>
+                      <c15:txfldGUID>{2F35FA20-6F16-4B11-836B-824CE340BCBB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$59</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19021,7 +19081,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D98C4B7A-64A3-4A3B-A96F-4E9ABDFA123D}</c15:txfldGUID>
+                      <c15:txfldGUID>{658A7757-CC7A-4994-83C1-03920AABC2F9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$60</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19062,7 +19122,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BC4625C2-18C4-4143-8881-4F6BBE837239}</c15:txfldGUID>
+                      <c15:txfldGUID>{879D7446-42CD-4D25-90AC-A3240EC7A56D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$61</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19103,7 +19163,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{637AE09A-19EF-442B-97FE-F6C047395600}</c15:txfldGUID>
+                      <c15:txfldGUID>{D3384808-55BE-4AEA-9506-D2B4F2F3F7AE}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$62</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19144,7 +19204,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C18E7AC9-0765-4A0D-A0B9-308B64D016DD}</c15:txfldGUID>
+                      <c15:txfldGUID>{1A83E9B1-F66B-4DDA-81C0-CBC2A7379071}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$63</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19185,7 +19245,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{984D5385-5992-4FBF-8EDF-611764C1F84C}</c15:txfldGUID>
+                      <c15:txfldGUID>{67B59771-58A6-4A55-A67A-A375CB86BAC2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$64</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19226,7 +19286,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AC0113DE-2ADB-4130-AAAA-D4E755BA207E}</c15:txfldGUID>
+                      <c15:txfldGUID>{9EA6ABE1-580B-46F2-B759-B47B72BCB34D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$65</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19267,7 +19327,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8A9A20D3-5696-4A4F-B95C-AFAD44A1E72B}</c15:txfldGUID>
+                      <c15:txfldGUID>{1FE13241-A91D-4FD1-B9F9-F84267096F3A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$66</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19308,7 +19368,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D887C9A1-534D-4851-9C6D-154429D15AE2}</c15:txfldGUID>
+                      <c15:txfldGUID>{3DE17338-CA07-4148-AE08-D72C68EDC546}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$67</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19349,7 +19409,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E01B9177-F40B-42C7-A318-5F41DAF39EBC}</c15:txfldGUID>
+                      <c15:txfldGUID>{A1BB7C57-0057-40BE-87FA-8B9653EB3649}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$68</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19390,7 +19450,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6AD37CFB-43C7-486B-8AAE-8E1086B2B2E5}</c15:txfldGUID>
+                      <c15:txfldGUID>{AFCD7038-DAC3-4E0E-8F85-078E54962E11}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$69</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19431,7 +19491,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{63DA7314-14E9-4806-9223-CCB03CE3CDF1}</c15:txfldGUID>
+                      <c15:txfldGUID>{F481F1E4-A415-4A65-8B71-5E1726B61F84}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19472,7 +19532,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{11999A9C-8C44-4781-99A3-DC775C1C9292}</c15:txfldGUID>
+                      <c15:txfldGUID>{625E60B2-ACDD-4467-A978-2A359005C7FD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$71</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19513,7 +19573,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{28630BC9-07BA-4B5C-968C-43DDD3F4FCC0}</c15:txfldGUID>
+                      <c15:txfldGUID>{3D5C4442-3766-48FC-8AAB-BE1E00A2F850}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19554,7 +19614,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0E3536C6-275D-458E-9812-7F3C8BDE2552}</c15:txfldGUID>
+                      <c15:txfldGUID>{390C2D00-E41C-4B66-9B9F-4004CC5DD79A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$73</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19595,7 +19655,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A520CBE6-D3F5-4FB6-96C7-419FED2893AF}</c15:txfldGUID>
+                      <c15:txfldGUID>{4BA8D786-424E-4EEE-8CA3-EADDDA8CCF0C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$74</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19636,7 +19696,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{999CBA52-61B2-46FD-9784-7C800579EE97}</c15:txfldGUID>
+                      <c15:txfldGUID>{679DB828-51B8-4A80-89F4-8E81DC3F2672}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$75</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19677,7 +19737,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FAEAC2B9-1623-43B6-A0FD-2A101A6A0220}</c15:txfldGUID>
+                      <c15:txfldGUID>{E2E8F93B-D2C0-4CD9-B2A8-DAC3FD0640D3}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$76</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19718,7 +19778,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E5D08633-958E-45C1-99CE-B71296CC5A1B}</c15:txfldGUID>
+                      <c15:txfldGUID>{32676891-A21E-4E65-A91F-2025EBF76F03}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$77</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19759,7 +19819,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{777CE949-3D94-46EA-85A0-8B46824085D7}</c15:txfldGUID>
+                      <c15:txfldGUID>{53742324-0D60-49CA-9CA4-C44BD5477B7C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$78</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19800,7 +19860,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{19E8B7F9-D53B-4425-A9ED-02F939E5F205}</c15:txfldGUID>
+                      <c15:txfldGUID>{7D4C47B3-8CAD-4342-A3C9-9C78D9BDCE08}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$79</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19841,7 +19901,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{504A120C-EAD4-4ED3-90CF-CECF30AD1C57}</c15:txfldGUID>
+                      <c15:txfldGUID>{09EC038F-FE2F-4AB2-A329-AA5BCDDAD4BD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$80</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19882,7 +19942,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{530528F3-5FCA-47B9-9591-95D527F02130}</c15:txfldGUID>
+                      <c15:txfldGUID>{D4EA7DE5-4FD4-4F37-B558-014808CE264B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$81</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19923,7 +19983,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FB2DBACF-38C2-4C0E-AACB-2DF016382F3E}</c15:txfldGUID>
+                      <c15:txfldGUID>{C016266C-B23E-4758-8076-0DDC3F4D8645}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$82</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -19964,7 +20024,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B00F3648-B244-4FA4-90D7-0B6424F8C5CC}</c15:txfldGUID>
+                      <c15:txfldGUID>{DB2070D8-0910-4198-B9EC-8150363C3450}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$83</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20005,7 +20065,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F2E0774B-CE99-41F0-87D9-BE8693EBE864}</c15:txfldGUID>
+                      <c15:txfldGUID>{697CA5B0-6F04-4933-B2CE-E1E693BBB5D0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$84</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20046,7 +20106,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{40BD8953-22C3-4E00-8AC6-51043088BFC3}</c15:txfldGUID>
+                      <c15:txfldGUID>{A2342DB4-7162-41AD-9BD0-40D0A80F2E33}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$85</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20087,7 +20147,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B55F89CD-5FEA-48FF-A6EF-271CF454522B}</c15:txfldGUID>
+                      <c15:txfldGUID>{13759F45-B457-435D-BF96-EF10F44E5CE4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$86</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20128,7 +20188,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{17234E38-7634-45F6-AD4D-A422715BD168}</c15:txfldGUID>
+                      <c15:txfldGUID>{201B29E7-345C-4238-8582-876D8C380E7E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$87</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20169,7 +20229,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0FBC1ADC-29B2-49B2-902C-27542FA672D3}</c15:txfldGUID>
+                      <c15:txfldGUID>{45E1B9EE-0F0E-43C2-8116-06C9BBE25072}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$88</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20210,7 +20270,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D55AF9A1-F937-4AB2-AC1F-5584B1540E87}</c15:txfldGUID>
+                      <c15:txfldGUID>{52417E05-1D3B-4122-9FA7-8AB59038CB31}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$89</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20251,7 +20311,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{83E1CD4C-5D95-43C5-ACD3-AD17584316BF}</c15:txfldGUID>
+                      <c15:txfldGUID>{A3D97272-A12F-40E4-BA29-145EF9266FD7}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$90</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20292,7 +20352,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E4E3D27D-2CDA-46AB-926F-4B7704E2B45D}</c15:txfldGUID>
+                      <c15:txfldGUID>{2E7A6C52-A77B-485D-90D7-C3C1834B4066}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$91</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20333,7 +20393,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{46E3DBDD-BD65-4B57-A5E2-B728C49CEF6B}</c15:txfldGUID>
+                      <c15:txfldGUID>{C9AE7EDD-2D78-4D6B-9596-58E4FB6CA492}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$92</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20374,7 +20434,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{57AEEAC8-2DA7-4BD5-87BA-027912FF5C4C}</c15:txfldGUID>
+                      <c15:txfldGUID>{85ECA044-4DD4-4104-9FBF-AE7ED5CE414C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$93</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20415,7 +20475,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C6F56E15-937D-4959-8EB5-C0D561B626BB}</c15:txfldGUID>
+                      <c15:txfldGUID>{2F2D2BD1-789C-4A1C-91D4-E206A850F87C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$94</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20456,7 +20516,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{52C89C67-64A9-4475-81B8-723390228F74}</c15:txfldGUID>
+                      <c15:txfldGUID>{C3D2AABE-812F-4FD5-B024-ACB41669B72F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$95</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20497,7 +20557,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{12062063-AF7F-4A4A-A796-B7437854DC91}</c15:txfldGUID>
+                      <c15:txfldGUID>{4E55420A-F642-46E8-B97F-94CBF3028A50}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$96</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20538,7 +20598,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E35372F3-88E2-48D6-980F-BE32FAF986EE}</c15:txfldGUID>
+                      <c15:txfldGUID>{B3460037-04B6-4ACD-9DBA-E545F6B0F4FB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$97</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20579,7 +20639,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2F5AD23D-3BB5-4EB5-ABEE-E163167F915A}</c15:txfldGUID>
+                      <c15:txfldGUID>{F7CFF0F4-51BC-41C8-92E4-7821E5378438}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$98</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20620,7 +20680,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{74672895-5611-4F8D-AA2F-C949E156A437}</c15:txfldGUID>
+                      <c15:txfldGUID>{E12C51DC-61DC-464D-9492-03C49B9D3960}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$99</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20661,7 +20721,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B8AFA7FF-4608-4F07-BCE8-5FEE707C1FFF}</c15:txfldGUID>
+                      <c15:txfldGUID>{2195CACE-512B-45FB-81F0-F9BD505AED90}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$100</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20702,7 +20762,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FB1D33AB-5811-415E-AA1E-B98582699DCA}</c15:txfldGUID>
+                      <c15:txfldGUID>{8F2D07FB-254D-4850-AC64-AAD2B2D66A7B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$101</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20743,7 +20803,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0E11BB02-3C3F-4A01-8C75-0176D225D772}</c15:txfldGUID>
+                      <c15:txfldGUID>{078691E2-A479-4E6D-8FD9-2552C0F72785}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$102</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20784,7 +20844,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6509974C-57A3-4395-9FC2-699C94265E9C}</c15:txfldGUID>
+                      <c15:txfldGUID>{F92ACDB6-67AA-4E52-A2F7-3349828401AE}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$103</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20825,7 +20885,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D4EF83C4-638A-418A-AD0C-2FB86A904EA7}</c15:txfldGUID>
+                      <c15:txfldGUID>{F78AB18E-86D0-46F3-9119-64EECAB0CA66}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$104</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20866,7 +20926,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0E038136-BE93-4AF5-8DF3-4A6F32D24737}</c15:txfldGUID>
+                      <c15:txfldGUID>{21CC8E80-865F-4F2B-98B5-BF90B9A5F75A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$105</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20907,7 +20967,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5A5E07ED-37D6-4BCF-BBF1-5FBCA3C58E8B}</c15:txfldGUID>
+                      <c15:txfldGUID>{C5172958-2538-4249-98C7-9CCEFBDADA55}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$106</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20948,7 +21008,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D7BBAFB9-5834-4436-8CCA-BF4D11C7BD33}</c15:txfldGUID>
+                      <c15:txfldGUID>{71E81024-F06D-4B98-8970-7D54408707F7}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$107</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -20989,7 +21049,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9839E081-BACC-47DD-9713-CB79B2D766E9}</c15:txfldGUID>
+                      <c15:txfldGUID>{12F4F866-A444-48AF-939E-46DD503E669A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$108</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21030,7 +21090,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BE2D6496-717F-4A04-B7BD-BE5CBB8DFA2E}</c15:txfldGUID>
+                      <c15:txfldGUID>{499B08BD-6441-4867-A127-BAA14EDCD3F1}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$109</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21071,7 +21131,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{00CCA67B-FA2E-47E3-92D4-F7D968E87DAC}</c15:txfldGUID>
+                      <c15:txfldGUID>{50D885EC-6066-4958-8B24-759E6EA90D89}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$110</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21112,7 +21172,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E83B1108-4C91-4CDB-A10B-60674B15F790}</c15:txfldGUID>
+                      <c15:txfldGUID>{4DB35FBD-5619-454E-904B-5CAD3631D376}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$111</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21153,7 +21213,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{90F0CD4F-1A96-4531-ABC3-E9A3E99E03DE}</c15:txfldGUID>
+                      <c15:txfldGUID>{8EE8973F-687B-42FE-A4F6-D34714692FE9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$112</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21194,7 +21254,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{07537002-8753-452E-9B76-C159B8B59542}</c15:txfldGUID>
+                      <c15:txfldGUID>{D7F9A0A3-0D5A-4FCC-8F5F-D1F1F89D83F8}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$113</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21235,7 +21295,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{141E2C4A-59BD-4FBB-BC05-41BC770A12F9}</c15:txfldGUID>
+                      <c15:txfldGUID>{4A4D5539-6C17-4FCD-BEB5-D42C4D6F1F5B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$114</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21276,7 +21336,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E9798772-F8B5-4DC3-938D-9D32230BAB08}</c15:txfldGUID>
+                      <c15:txfldGUID>{0FF314B4-5A71-4976-A36B-64AA92B92728}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$115</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21317,7 +21377,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F1B583A8-314D-48A0-B0FA-4C8EFB6C5F3E}</c15:txfldGUID>
+                      <c15:txfldGUID>{14D444DD-14D6-4295-973A-84F521D15067}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$116</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21358,7 +21418,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9FD0FE0F-D7C7-4F5C-ABD4-C4A693FC5A7E}</c15:txfldGUID>
+                      <c15:txfldGUID>{89EF4F32-64B0-482F-A9E9-EBFBF47833DB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$117</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21399,7 +21459,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A1E4A719-0B07-4183-858D-6509AD86C084}</c15:txfldGUID>
+                      <c15:txfldGUID>{6D3B4437-5B60-4FE9-8496-1767360CF3C1}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$118</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21440,7 +21500,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7F4F39E7-2FE7-4067-B47A-308797CFC68A}</c15:txfldGUID>
+                      <c15:txfldGUID>{63A92D53-57D0-4EC1-9008-D028B4140FEB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$119</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21481,7 +21541,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E86F7171-7B24-4DA9-A0B6-EF1CBC3F8EC7}</c15:txfldGUID>
+                      <c15:txfldGUID>{D0680DEA-1579-4795-BE73-BE37B5B73BD2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$120</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21522,7 +21582,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4CE3E1C1-E58D-4822-82EF-FCB98B64C9AF}</c15:txfldGUID>
+                      <c15:txfldGUID>{2C182DD1-A602-4AAA-B661-F998AAE3F084}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$121</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21563,7 +21623,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C1688E45-25F9-439E-9DCA-39C9F74DA6FB}</c15:txfldGUID>
+                      <c15:txfldGUID>{C23DA133-3BA3-4BAD-A50A-AC2BAF5586A3}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$122</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21604,7 +21664,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{50335638-552C-42AE-ADDC-1C59E5A3526F}</c15:txfldGUID>
+                      <c15:txfldGUID>{1CBF9149-B170-4B49-A199-BC37775C43E6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$123</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21645,7 +21705,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4F1ACD96-3C74-4D58-894B-B7F884D60FDC}</c15:txfldGUID>
+                      <c15:txfldGUID>{74821D79-DD32-428A-926D-3A2AA7038570}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$124</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21686,7 +21746,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3A9624B7-E65E-4796-A138-5F44689EBD40}</c15:txfldGUID>
+                      <c15:txfldGUID>{BE6A4266-88B6-4674-9561-ADCE59016BE5}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$125</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21727,7 +21787,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{72A5C073-2E5C-4B44-AA0C-B449E1759497}</c15:txfldGUID>
+                      <c15:txfldGUID>{ACBF84FA-0877-4BB3-9911-7FFF570D93E2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$126</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21768,7 +21828,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AE3536ED-C715-4BF5-8422-1E730D86F04F}</c15:txfldGUID>
+                      <c15:txfldGUID>{06A5D5AA-CBB2-4D57-AEFE-76E3917E1704}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$127</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21809,7 +21869,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4A9E6D74-A664-4831-90ED-882C0E3C176A}</c15:txfldGUID>
+                      <c15:txfldGUID>{603B2828-11CC-4512-B494-5892A31358F0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$128</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21850,7 +21910,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{68DA5624-A1C2-4CB2-935B-155DE97DAEB2}</c15:txfldGUID>
+                      <c15:txfldGUID>{8E4DBFE5-B78C-47D0-80FE-454BC549633F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$129</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21891,7 +21951,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{652DD80E-9F53-4C30-B84B-E6B1F5EAD9F9}</c15:txfldGUID>
+                      <c15:txfldGUID>{0AD51223-3599-4B9A-ADA4-D1DD6CE3CFB9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$130</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21932,7 +21992,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{52AD0E93-5E61-4E6B-BEF3-650AE8D009F4}</c15:txfldGUID>
+                      <c15:txfldGUID>{254A4EE8-8F6E-4F72-B16B-93E58B6A500D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$131</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -21973,7 +22033,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{08168A9C-4FFA-46B0-8EA9-F62B47716543}</c15:txfldGUID>
+                      <c15:txfldGUID>{CFE4A151-5B28-41E1-BF86-888F02FFE292}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$132</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22014,7 +22074,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{587C5703-A6E2-4DB7-A10E-DA6FA709413E}</c15:txfldGUID>
+                      <c15:txfldGUID>{EBB45055-5CC8-404F-91AF-B072E88836F9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$133</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22055,7 +22115,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E2FA5878-BA6A-406C-8EB1-EF3FB6C0393C}</c15:txfldGUID>
+                      <c15:txfldGUID>{652B4E80-996B-4FE9-A842-C4FE0773760B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$134</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22096,7 +22156,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3292372A-139A-429A-8FE2-6AF193D1B45D}</c15:txfldGUID>
+                      <c15:txfldGUID>{28B37CA3-079E-416E-8324-0A4923577E1B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$135</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22137,7 +22197,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D23D2850-C157-4995-858E-40B2B832B7F9}</c15:txfldGUID>
+                      <c15:txfldGUID>{F334B3EA-3544-4FF5-96B3-5CF1D132113E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$136</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22178,7 +22238,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E114BB6D-4DAF-4310-8C6D-764D09EB8BF2}</c15:txfldGUID>
+                      <c15:txfldGUID>{84D1AF10-6180-419D-BCB3-2015E638D97E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$137</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22219,7 +22279,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{13A1B1DF-96D7-4384-9B22-47CD02DD10C4}</c15:txfldGUID>
+                      <c15:txfldGUID>{DF359DA0-A17B-4481-B029-A0EC703F52CA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$138</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22260,7 +22320,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{38A83DBC-DEBD-44E0-B8E0-32BA83A015E3}</c15:txfldGUID>
+                      <c15:txfldGUID>{92E54645-B41B-4472-9CA2-8EF2C87639A7}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$139</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22301,7 +22361,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EA163BE6-2689-4F3C-9463-092B72B4C64E}</c15:txfldGUID>
+                      <c15:txfldGUID>{3634F1D1-24EF-4C48-A68E-666131C72560}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$140</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22342,7 +22402,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B2ECC93A-9181-445C-9B8A-E60A6D6332A4}</c15:txfldGUID>
+                      <c15:txfldGUID>{8B608665-1A4A-4627-B3B6-C0DFD58FE5ED}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$141</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22383,7 +22443,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1E528D61-D5F5-4613-BBEC-58395EB778EB}</c15:txfldGUID>
+                      <c15:txfldGUID>{9922319F-A27F-49B0-9E60-1B3800001F58}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$142</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22424,7 +22484,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8BAB5FA9-4C7B-4A6D-B70B-2B22B28DBEF4}</c15:txfldGUID>
+                      <c15:txfldGUID>{F809FD71-F264-49BB-ACFE-BE6513F38F24}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$143</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22465,7 +22525,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{35406C25-206E-4CFA-B72B-A6D2579FEAEE}</c15:txfldGUID>
+                      <c15:txfldGUID>{CFEA4FB4-B386-4D27-B9AF-546DC1FB0BC0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$144</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22506,7 +22566,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{502B47EB-FBC0-433F-B9F4-42F1ACC54090}</c15:txfldGUID>
+                      <c15:txfldGUID>{F1F40E90-C719-457A-9079-7793EFA9F74D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$145</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22547,7 +22607,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{681B1613-82CD-431F-817B-2F4D4FF82D1B}</c15:txfldGUID>
+                      <c15:txfldGUID>{A55791AD-A89D-4B81-87D5-12DABC0D7800}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$146</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22588,7 +22648,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BBF4C387-F850-49FF-9846-0ECA63ADE6C9}</c15:txfldGUID>
+                      <c15:txfldGUID>{FE4431B2-FFAB-44BE-BBAF-C0D8E4E2472C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$147</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22629,7 +22689,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9A327747-47E9-4A20-8575-FE8AA4F9AC6E}</c15:txfldGUID>
+                      <c15:txfldGUID>{2A00CD9F-D3D2-4E5F-9249-ACDECA2E53E0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$148</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22670,7 +22730,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{406EC729-570C-4271-94A7-9AFC80C3006D}</c15:txfldGUID>
+                      <c15:txfldGUID>{F1BB9E84-176E-4D27-A8B7-D5D9C8E88C6F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$149</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22711,7 +22771,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{97162430-F048-4FA3-93FD-51B4B62B393F}</c15:txfldGUID>
+                      <c15:txfldGUID>{4D3314A3-F657-4DFD-8D4D-AFCB3D98775F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$150</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22752,7 +22812,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D2F8F24A-2FDA-411D-A8A1-F92EDB54B38F}</c15:txfldGUID>
+                      <c15:txfldGUID>{59DF106D-039C-4AF9-93B5-9D997B75067A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$151</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22793,7 +22853,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{876C2412-31C5-43C6-A98B-CAD2C1F1B9BA}</c15:txfldGUID>
+                      <c15:txfldGUID>{4DB3B666-63DE-421B-BB45-AD72AA4659FB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$152</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22834,7 +22894,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4293BBD7-B177-44DD-BCD3-8D9EF32EFA09}</c15:txfldGUID>
+                      <c15:txfldGUID>{83DB7774-D565-4DF4-B7A5-42CB78570438}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$153</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22875,7 +22935,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{ABE3C031-19A7-4FEB-8590-B6D57A2C542A}</c15:txfldGUID>
+                      <c15:txfldGUID>{B94551DC-450E-4A4A-8E89-2329C2F382E2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$154</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22916,7 +22976,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9FCABCF0-ED12-4D55-AF4F-C63F835A8D6E}</c15:txfldGUID>
+                      <c15:txfldGUID>{6C9BBE9B-7EA2-4E07-9BAF-C15D2AA595D6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$155</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22957,7 +23017,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{64F35E9C-6FF7-4EC7-BCEE-333F0EE9CEF8}</c15:txfldGUID>
+                      <c15:txfldGUID>{6E1600BE-9F04-4A95-8624-04868908679B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$156</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -22998,7 +23058,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0654A9D1-BD29-4598-AC77-50F99A1C93FF}</c15:txfldGUID>
+                      <c15:txfldGUID>{24078E55-A722-413B-A507-A7C38972F601}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$157</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23039,7 +23099,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8F137035-14E5-4C18-82E9-E9FBFE3703FB}</c15:txfldGUID>
+                      <c15:txfldGUID>{12A2B938-F755-42ED-9B56-FB6D9D20D056}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$158</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23080,7 +23140,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5C9C9FCD-27C4-49B1-813E-6E2655D83DB5}</c15:txfldGUID>
+                      <c15:txfldGUID>{5C094112-C8B5-4FBE-BEE9-7E9F728BF76D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$159</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23121,7 +23181,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F04D4394-45AF-4266-9487-6BF1B60B7095}</c15:txfldGUID>
+                      <c15:txfldGUID>{4AA9FA2E-5632-4F61-9B63-AD6C6EC6DEA7}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$160</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23162,7 +23222,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{599D9B17-B755-4B06-8D23-AFD353F735DD}</c15:txfldGUID>
+                      <c15:txfldGUID>{5B2D62E6-F9ED-4D34-8E17-C3155E5693D4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$161</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23203,7 +23263,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0CFE1D4B-B9D5-44E1-B72A-E5F47359BC10}</c15:txfldGUID>
+                      <c15:txfldGUID>{5E31C9A8-F9CE-4447-B5EC-C908E03EDA1D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$162</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23244,7 +23304,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DC162A9C-A7A4-46F8-AC0A-14EBC53DFCAC}</c15:txfldGUID>
+                      <c15:txfldGUID>{03B37AD4-3476-4CD8-8FE5-9C5C7A784559}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$163</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23285,7 +23345,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9F5784FA-AD1F-4170-86A3-3603A93D922A}</c15:txfldGUID>
+                      <c15:txfldGUID>{51D53B3C-E46E-4AD7-B891-D3EA5D35457D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$164</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23326,7 +23386,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3E272F56-AFB2-472A-A306-1B67A84B09C7}</c15:txfldGUID>
+                      <c15:txfldGUID>{133E38D1-FAC2-4A2B-BCCC-0B07EA30B1E1}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$165</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23367,7 +23427,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3AEDA1CB-CE6F-4236-BECD-9A4B525874CA}</c15:txfldGUID>
+                      <c15:txfldGUID>{7EFBEBFE-3084-4D5C-97C1-BC4E78646EEA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$166</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23408,7 +23468,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4F04DC27-1AAF-42A6-8F43-9E14886C77AE}</c15:txfldGUID>
+                      <c15:txfldGUID>{2125FE2B-C885-41AC-AB34-BD8F77467F03}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$167</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23449,7 +23509,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2060CE72-A5B9-4C50-ABA0-CF268D82D293}</c15:txfldGUID>
+                      <c15:txfldGUID>{1800A33E-7A49-465F-BA3B-9B4CB4F082E0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$168</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23490,7 +23550,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{29C2130A-8879-46DA-AFD5-72251548CED8}</c15:txfldGUID>
+                      <c15:txfldGUID>{0C71CB25-B87D-4AEF-A959-9D9E6B7B4376}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$169</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23531,7 +23591,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C68DA137-D8B2-49B9-8648-B18318D668DE}</c15:txfldGUID>
+                      <c15:txfldGUID>{9464F1E1-63FF-4779-A711-499B402E6498}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$170</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -23576,10 +23636,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$E$2:$E$253</c:f>
+              <c:f>'Bill Data'!$E$2:$E$254</c:f>
               <c:numCache>
                 <c:formatCode>0\°</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>69</c:v>
                 </c:pt>
@@ -24335,16 +24395,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$T$2:$T$253</c:f>
+              <c:f>'Bill Data'!$T$2:$T$254</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>0.20833333333333334</c:v>
                 </c:pt>
@@ -25100,6 +25163,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>0.25806451612903225</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25243,7 +25309,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C5F326B6-7C3E-4CA5-9B20-8FF5465F7DAA}</c15:txfldGUID>
+                      <c15:txfldGUID>{6012BF03-692D-4CD7-934D-1D670EBB8DBC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$2</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25284,7 +25350,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{09A0C539-EFEA-4D40-B366-B3532D10BCF2}</c15:txfldGUID>
+                      <c15:txfldGUID>{60E2E86B-E198-4760-B945-6955DC04756A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$3</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25325,7 +25391,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5F13F04F-43F3-495A-8EF0-8D46A6ADFDA8}</c15:txfldGUID>
+                      <c15:txfldGUID>{FA4BC3B1-4F29-4B98-8582-78FF3D973132}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$4</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25366,7 +25432,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{01F1DD92-FF64-4A35-80F9-6DFA18A5787F}</c15:txfldGUID>
+                      <c15:txfldGUID>{24C6050C-83A2-408E-9ACF-9ECDDC73F159}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25407,7 +25473,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C10173D9-C103-4B8C-9FB7-A89820EF126E}</c15:txfldGUID>
+                      <c15:txfldGUID>{F00B35B1-692C-4E2B-A84F-1E00EC937799}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$6</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25448,7 +25514,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8839F8F1-C84F-4ACF-AA2E-7CB170F69CCE}</c15:txfldGUID>
+                      <c15:txfldGUID>{1F69E891-F30E-42AF-A0B7-38A980BC27D9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$7</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25489,7 +25555,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{652C94FF-CF51-44ED-B41E-F5B6BDC67898}</c15:txfldGUID>
+                      <c15:txfldGUID>{54AEAD70-C2DA-425C-A929-4E1F06E5CA33}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$8</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25530,7 +25596,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6D685144-B198-45FA-9C5C-D681C100477A}</c15:txfldGUID>
+                      <c15:txfldGUID>{761EE808-19D2-4043-BA29-458728D7F5E9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$9</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25571,7 +25637,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A2D32B5B-2945-47A6-8FC0-1B02B06AB732}</c15:txfldGUID>
+                      <c15:txfldGUID>{29F49C7D-B5C5-40B0-BFE5-7A21F3CD7020}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$10</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25612,7 +25678,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3F18BB8C-F9F0-4EB9-9FAE-5292AFBEE2A7}</c15:txfldGUID>
+                      <c15:txfldGUID>{69BE6BAB-D3E2-42F0-8833-F24C17C04044}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$11</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25653,7 +25719,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B58A2716-D818-4C9E-B064-259141B3CD90}</c15:txfldGUID>
+                      <c15:txfldGUID>{6F3A03D1-069C-4373-A78B-ADBAD1ED6DED}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$12</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25694,7 +25760,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1F248D39-C32A-4E7C-BDB4-1D7E719131FA}</c15:txfldGUID>
+                      <c15:txfldGUID>{2F6FE6B5-EBF4-4536-B079-9AF4F24B4D64}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$13</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25735,7 +25801,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5BAD1518-679F-44BD-8C00-3E56347FEDF2}</c15:txfldGUID>
+                      <c15:txfldGUID>{C0601FE4-7987-4644-8886-CB8B0BE02705}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$14</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25776,7 +25842,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DE9F4F04-F452-43A5-B964-EC3192FEC46B}</c15:txfldGUID>
+                      <c15:txfldGUID>{899C3554-0258-4C01-ABDB-72592CAF2A95}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$15</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25817,7 +25883,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F8DFDC33-6101-4550-B1A0-360CC30399C1}</c15:txfldGUID>
+                      <c15:txfldGUID>{B1C1EEBB-AB9F-49B0-8558-418CFFDFF748}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$16</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25858,7 +25924,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{57468781-79FC-4FEB-B219-7E33A7390C68}</c15:txfldGUID>
+                      <c15:txfldGUID>{666CEB1A-916C-411A-A0FB-294FFB1E6110}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$17</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25899,7 +25965,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6243E2B0-77A7-44E4-A6A2-725DA0DEAC29}</c15:txfldGUID>
+                      <c15:txfldGUID>{64873530-34B3-4716-9C2F-02FE50F5FD2A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$18</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25940,7 +26006,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{65652B77-7EA4-4971-B07F-E86203E914AB}</c15:txfldGUID>
+                      <c15:txfldGUID>{DD3AB12E-C0A4-4BB5-ABDB-F6B46FEBEB22}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$19</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -25981,7 +26047,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FF9A36D1-7549-40F0-AAAD-D74F6F2DD795}</c15:txfldGUID>
+                      <c15:txfldGUID>{246E8A38-839C-4816-B006-CCF3F64278D2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$20</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26022,7 +26088,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A6C6925F-CECE-4CC4-9CA0-F2FC4679D1C9}</c15:txfldGUID>
+                      <c15:txfldGUID>{D7743093-FEFD-4B68-BB46-E7875D060DD1}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$21</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26063,7 +26129,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4E9280F4-8EC1-4303-9CC4-5DB8F9058FCA}</c15:txfldGUID>
+                      <c15:txfldGUID>{4837C19C-944D-47A6-91CE-05F65E314774}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$22</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26104,7 +26170,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8FAC78C6-5075-4305-A8E2-56B86A2C7AC6}</c15:txfldGUID>
+                      <c15:txfldGUID>{61D7956D-EB9D-4AF0-8A4D-D308FE94572D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$23</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26145,7 +26211,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{054EF8BC-5804-491F-93FA-33D1FAC67E9E}</c15:txfldGUID>
+                      <c15:txfldGUID>{8EADA910-845D-4D09-9B46-F901B87348F5}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$24</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26186,7 +26252,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A869F4C9-7609-4098-95BA-2B35D52BEDFA}</c15:txfldGUID>
+                      <c15:txfldGUID>{C9F51F6B-7A6A-4740-B43D-3BE9B995DD98}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$25</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26227,7 +26293,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{26B332A4-1D0D-49D0-BC48-E3AF9318485C}</c15:txfldGUID>
+                      <c15:txfldGUID>{B3D65310-830B-4524-B03C-7EB045D398FF}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$26</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26268,7 +26334,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{40A79DA8-A396-4DFA-9A4C-7D5DEC0E0AB6}</c15:txfldGUID>
+                      <c15:txfldGUID>{C267D91D-B4A7-4E8B-9245-A71BBDD9027D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$27</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26309,7 +26375,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E1BF046D-77E7-4617-8BCF-A03F0DB4C1A9}</c15:txfldGUID>
+                      <c15:txfldGUID>{38A6F99A-1030-46C4-B906-33CD5596D797}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$28</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26350,7 +26416,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F94A99F4-B6FE-4F1D-8762-08490945D769}</c15:txfldGUID>
+                      <c15:txfldGUID>{695C8DA1-054E-4A9D-850A-055B37FDA7D0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$29</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26391,7 +26457,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FA2F9054-45C8-4B2F-9221-1E67A8C246C0}</c15:txfldGUID>
+                      <c15:txfldGUID>{333EB2FF-3148-4263-BA36-39E2B1168FBF}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$30</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26432,7 +26498,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{834756BD-71F3-43DB-A72C-8ABB1DF3250A}</c15:txfldGUID>
+                      <c15:txfldGUID>{5A18DA3A-F749-4B59-AA09-4E71DAFAD8FA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$31</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26473,7 +26539,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E438A204-FA59-4CF5-B934-C38A5CCD545E}</c15:txfldGUID>
+                      <c15:txfldGUID>{6B56EF2E-4020-4AE3-84CB-2647F82840A9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$32</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26514,7 +26580,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C086BEE4-4B73-4059-8692-397FE7B44A86}</c15:txfldGUID>
+                      <c15:txfldGUID>{DDEC11C7-8D87-4AE6-8217-8280DC333A6F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$33</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26555,7 +26621,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C268657A-C37F-4D43-948A-CBC180F23319}</c15:txfldGUID>
+                      <c15:txfldGUID>{4FB08846-7209-48C5-9013-3FF64CE32E38}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$34</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26596,7 +26662,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8EE0FAE6-5117-4B45-9AB5-6968B3966582}</c15:txfldGUID>
+                      <c15:txfldGUID>{2EF95E0F-9D06-47B8-83C1-5D57AB56AD2D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$35</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26637,7 +26703,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{10D9DAE8-7FE0-4ACE-8991-E6C28D5E5362}</c15:txfldGUID>
+                      <c15:txfldGUID>{803FBF33-2536-4614-A93C-88568BEA72E8}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$36</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26678,7 +26744,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BDD99032-B035-4E7F-9214-72A7EF4601C6}</c15:txfldGUID>
+                      <c15:txfldGUID>{085B2ABA-0D4A-4DA0-A53F-3ADC189090D3}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$37</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26719,7 +26785,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{89B60C2C-781E-43F5-B318-76731F73EEA5}</c15:txfldGUID>
+                      <c15:txfldGUID>{AEFD1B1F-B6F7-4C37-94C7-35D08F0F0017}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$38</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26760,7 +26826,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5AFB7FCE-D7A0-4DEA-A51F-69055B01A023}</c15:txfldGUID>
+                      <c15:txfldGUID>{6378949A-8221-4461-BAF3-F452A5CBDE15}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$39</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26801,7 +26867,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6236EF77-11D7-4FD8-8791-5A59E6A74AD6}</c15:txfldGUID>
+                      <c15:txfldGUID>{18CA3451-722A-441A-B235-561A27A643AC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$40</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26842,7 +26908,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{295C796F-8FE0-43B7-8B4F-020CD7E9DDA7}</c15:txfldGUID>
+                      <c15:txfldGUID>{3B2E9EC7-A31A-42BB-B348-7F9A3E2BBF9C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$41</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26883,7 +26949,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{00F57654-3CFC-4B24-9052-F01BA4CE5CF0}</c15:txfldGUID>
+                      <c15:txfldGUID>{9F9E7E4B-2AD9-49EE-B13F-DA3D2F156043}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$42</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26924,7 +26990,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8F5FA23A-90DC-4073-85E5-ADE107ABAD5A}</c15:txfldGUID>
+                      <c15:txfldGUID>{3EB8B977-C643-4A64-871A-624147D68786}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$43</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -26965,7 +27031,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{80D6291E-483F-4903-8CF1-40C0ADBAFA85}</c15:txfldGUID>
+                      <c15:txfldGUID>{69D81634-2831-4B9E-BA31-CC408EAF098F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$44</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27006,7 +27072,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{090F23BC-6D4E-4323-8C45-D426635FBF22}</c15:txfldGUID>
+                      <c15:txfldGUID>{087C192A-674A-4827-83C5-A6BA4B8AE2A4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$45</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27047,7 +27113,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3F1FAC6D-CDE3-4892-83D9-C9FC921A4E0E}</c15:txfldGUID>
+                      <c15:txfldGUID>{97FB7CB3-AD09-4453-9440-2D70224CD23C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$46</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27088,7 +27154,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{779D7BCF-CFE9-41BC-BA5D-958234D2DFB5}</c15:txfldGUID>
+                      <c15:txfldGUID>{39BF7963-3C3B-44E1-B30D-44B2E32CE344}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$89</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27129,7 +27195,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5FDE8ED4-2F82-496B-BCF4-8DA4396652FD}</c15:txfldGUID>
+                      <c15:txfldGUID>{EE02B16A-3826-408E-8143-EFEBF27B2B3B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$90</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27170,7 +27236,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C4B6FF98-916E-4BA8-A5F8-DBA070A7C807}</c15:txfldGUID>
+                      <c15:txfldGUID>{B94692B8-E14E-47C1-8640-9BDAFC5CAC87}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$91</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27211,7 +27277,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AAE08017-EEB4-4368-9AF9-0E34F629F18B}</c15:txfldGUID>
+                      <c15:txfldGUID>{F3E431F5-6F49-4D28-9C06-2B239B488E83}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$92</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27252,7 +27318,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A531374E-C2F4-4426-820C-62A4D75DC624}</c15:txfldGUID>
+                      <c15:txfldGUID>{0DF2DBC2-37FC-44C4-82C9-9413BBD5A984}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$93</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27293,7 +27359,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8292730A-3D0B-48AE-9C23-0244DF46E464}</c15:txfldGUID>
+                      <c15:txfldGUID>{9A840697-F757-457A-85F4-A13DFE5B5DDA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$94</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27334,7 +27400,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{29F2B824-920F-4AFC-A1C6-BE9A833789A6}</c15:txfldGUID>
+                      <c15:txfldGUID>{E1222758-B794-45E0-82B5-5A322840C2F8}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$95</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27375,7 +27441,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9836DC04-4E90-48BB-8E0A-89A1DD3C67F1}</c15:txfldGUID>
+                      <c15:txfldGUID>{216E551F-655C-4757-B3A2-3E326077C78B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$96</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27416,7 +27482,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FFF6401A-EC2F-4BE2-8A0D-28F4BCB47C9D}</c15:txfldGUID>
+                      <c15:txfldGUID>{A0FE5317-166C-405D-AFB9-53CE654511B9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$97</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27457,7 +27523,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B3297F56-A4C4-47C5-A4F4-C2941E3A36B0}</c15:txfldGUID>
+                      <c15:txfldGUID>{7CF72656-CFC0-4199-ABCE-9A34AC016DA6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$98</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27498,7 +27564,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{473D7A1D-40B3-4797-BF0A-EFBEFAD7A85A}</c15:txfldGUID>
+                      <c15:txfldGUID>{83689C7C-CBA5-4EC8-9FD2-FA309CF76E0C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$99</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27539,7 +27605,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8A94E0BB-51B1-4492-B74E-B858F08691A2}</c15:txfldGUID>
+                      <c15:txfldGUID>{E4F40F7A-0078-455A-BFE2-7DF94577167C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$100</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27580,7 +27646,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E9B31DE0-34C8-4F99-A01E-4B2EB29C9221}</c15:txfldGUID>
+                      <c15:txfldGUID>{90316CAB-1130-4501-8DFA-7AE846776C09}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$101</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27621,7 +27687,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{06017C07-72A5-4EAC-BD9C-B7135A416E1D}</c15:txfldGUID>
+                      <c15:txfldGUID>{93FF5F1E-AFBD-4D5E-93F6-E643C6D0FF96}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$102</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27662,7 +27728,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7D1B7154-4F38-4620-9A07-BD95B0B14861}</c15:txfldGUID>
+                      <c15:txfldGUID>{9009FC39-551F-4E1E-B01A-E2FEA779A36C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$103</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27703,7 +27769,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{18B14270-1386-4EA1-8DF2-00B15BAA2DBE}</c15:txfldGUID>
+                      <c15:txfldGUID>{56ACCC8F-4F43-4A58-8F28-AB9C228D27A2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$104</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27744,7 +27810,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{71EC9A06-4271-4F16-BADF-9A7057CB8E58}</c15:txfldGUID>
+                      <c15:txfldGUID>{C24C7FA0-D24F-4F31-BD34-72F12862BDB3}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$105</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27785,7 +27851,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7CB8E462-6307-4761-96D8-7A2420E82079}</c15:txfldGUID>
+                      <c15:txfldGUID>{4FB4F47F-158E-47C1-A1D6-9BBB862890A4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$106</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27826,7 +27892,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{75BCC0A7-159F-4398-B78A-CE21EEEFF0B4}</c15:txfldGUID>
+                      <c15:txfldGUID>{233FB21F-0B64-4633-8976-924C5121C81C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$107</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27867,7 +27933,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D11B2ACF-A938-45E5-A4D9-DA752DA53B54}</c15:txfldGUID>
+                      <c15:txfldGUID>{E233A747-17C8-4F85-9FFC-6DF8C27924F3}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$108</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27908,7 +27974,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{ED170794-3C90-41D9-B700-7EB93B3FC35E}</c15:txfldGUID>
+                      <c15:txfldGUID>{4EE724DD-4FA6-40A1-BDCB-7A6BCEBD6AA2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$109</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27949,7 +28015,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{646CEED0-C0E2-4783-9794-846B81A79FB3}</c15:txfldGUID>
+                      <c15:txfldGUID>{3215C065-DA97-4C5A-B26A-EB1C5C5CE978}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$110</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -27990,7 +28056,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5090A425-2E87-4E4C-83B7-82FAB0179D11}</c15:txfldGUID>
+                      <c15:txfldGUID>{9C4630E8-FCFC-4312-9AEB-62CD52422C09}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$111</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28031,7 +28097,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3C0BA5C5-DABC-4D8C-A778-C7FD7DA4C487}</c15:txfldGUID>
+                      <c15:txfldGUID>{444B08B6-FE56-4EB4-B09C-89E2FDDD098D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$112</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28072,7 +28138,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{357F6763-70C7-41A5-BEB4-E54F741CE5F8}</c15:txfldGUID>
+                      <c15:txfldGUID>{CCAD865F-EDD5-43CD-B6E5-CD0F6ADD1E1E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$113</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28113,7 +28179,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{28110CF9-658A-44A0-959D-4AE19970408C}</c15:txfldGUID>
+                      <c15:txfldGUID>{05F850BA-8843-4E43-8796-9E90789DE901}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$114</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28154,7 +28220,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C0273BE2-A79C-4D32-990C-AD926FD7BE67}</c15:txfldGUID>
+                      <c15:txfldGUID>{3215F531-9F2F-4464-B912-86F1A2C8C7BE}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$115</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28195,7 +28261,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CEA2E5F7-76C0-46D5-9C01-EBB802C4EB72}</c15:txfldGUID>
+                      <c15:txfldGUID>{79F681F9-AFC5-4207-858C-379F813D6E11}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$116</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28236,7 +28302,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C7B20134-64C5-465C-A2F1-33BDA09E5721}</c15:txfldGUID>
+                      <c15:txfldGUID>{F51227AA-5B3C-4AA5-8EA7-6CDC34C3C52B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$117</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28277,7 +28343,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D91B6EAA-B9B3-4441-93B8-53825EBD5182}</c15:txfldGUID>
+                      <c15:txfldGUID>{C0A717D5-C01F-4A00-B9C0-9A413B50C25E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$118</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28318,7 +28384,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D00F4A62-2050-4416-96F4-183D95A4A668}</c15:txfldGUID>
+                      <c15:txfldGUID>{106FA8AA-5914-45E7-BA89-C5A58B5E3647}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$119</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28359,7 +28425,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FCA5481A-DE6F-49C6-9385-E1619B259987}</c15:txfldGUID>
+                      <c15:txfldGUID>{6AC5A483-7ADE-42CD-B11C-1244CD811B66}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$120</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28400,7 +28466,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C2E80122-4C9F-4569-81FA-E5C47127C76D}</c15:txfldGUID>
+                      <c15:txfldGUID>{98BDC924-8AB6-4E07-B76A-4CC3C60BB23E}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$121</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28441,7 +28507,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{56574C87-C807-4B2A-8154-5FCA275EB831}</c15:txfldGUID>
+                      <c15:txfldGUID>{1B58831F-989A-43CF-B36E-0E29F8E0B3B9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$122</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28482,7 +28548,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{47806220-F65C-4E83-9699-0D27DC7FF9CA}</c15:txfldGUID>
+                      <c15:txfldGUID>{B4E4434F-68B0-4574-AED5-CDA1BD2C3751}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$123</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28523,7 +28589,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{226C514F-D810-4D59-A608-DBBE37B8B968}</c15:txfldGUID>
+                      <c15:txfldGUID>{6E95580C-825E-4763-BC49-9F969153E0D5}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$124</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28564,7 +28630,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8511E39D-DB77-4B53-9516-DE72AC8C2524}</c15:txfldGUID>
+                      <c15:txfldGUID>{8FF50125-8BAD-4572-800F-AE0D18D0A9DC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$125</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28605,7 +28671,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B23D9261-240E-43AE-8B7A-9A1A8CC3F7F2}</c15:txfldGUID>
+                      <c15:txfldGUID>{BEBCB5A7-79F0-431A-968C-C2B9BE13FC9D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$126</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28646,7 +28712,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B8E56EC2-8BDA-44B7-9944-AD6CF65D7A13}</c15:txfldGUID>
+                      <c15:txfldGUID>{DAD01079-FADF-415A-B6D7-6FD3126025FB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$127</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28687,7 +28753,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E8783EB0-DF41-4C04-8721-00A64AC8F067}</c15:txfldGUID>
+                      <c15:txfldGUID>{2EB2FADA-74BF-4F2D-AB72-11591E2594FC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$128</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28728,7 +28794,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3E9CE761-E80E-4936-B40E-22FA5DF5143C}</c15:txfldGUID>
+                      <c15:txfldGUID>{D7C7DBB8-5B3F-426C-A334-E5FE80C76FEA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$129</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28769,7 +28835,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7DF340A3-F888-4B33-B642-8D2F3BD76AAF}</c15:txfldGUID>
+                      <c15:txfldGUID>{BFD17149-ECD1-4373-9AC1-519235370534}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$130</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28810,7 +28876,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A1B6AF61-D3EE-40B2-867A-8122DAD1FBDA}</c15:txfldGUID>
+                      <c15:txfldGUID>{9EC0D454-F9D7-400F-BF45-CF7BE3F026FC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$131</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28851,7 +28917,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{60A62F18-63F2-4123-BF05-EF905835E3A1}</c15:txfldGUID>
+                      <c15:txfldGUID>{BE88D382-215C-4260-86FF-730993BB606F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$132</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28891,7 +28957,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C9745EC0-D273-4D3D-9765-3AAFB428A773}</c15:txfldGUID>
+                      <c15:txfldGUID>{4790DA1E-466E-43BD-9907-28345613FC18}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$133</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28931,7 +28997,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B26547F9-8175-403E-8F47-901F1D0B00D4}</c15:txfldGUID>
+                      <c15:txfldGUID>{0E5A3232-CF0A-414B-A8E4-F83FC1A81444}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$134</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -28971,7 +29037,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BA104359-EE27-4E92-A58D-C0B2DEFC3846}</c15:txfldGUID>
+                      <c15:txfldGUID>{51CCC9AD-6C9D-495B-A920-D8107A0078F1}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$135</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29011,7 +29077,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D566C475-F72F-49A3-8C94-5BF7D4BD429E}</c15:txfldGUID>
+                      <c15:txfldGUID>{F2B56A0F-568B-4908-9B08-3D2E90CB9911}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$136</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29051,7 +29117,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{97146648-B201-4FC8-A015-CE5B11B4A34C}</c15:txfldGUID>
+                      <c15:txfldGUID>{EC13266E-1BF8-4992-AE65-4C6F7BD90DC6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$137</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29091,7 +29157,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6B99E207-FF8C-49DA-A123-14DC12D8FEA5}</c15:txfldGUID>
+                      <c15:txfldGUID>{8971885A-9FDE-4ED8-A8FB-3B6749C1F469}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$138</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29131,7 +29197,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9A5058D7-270C-4BFD-B552-EA11E7904A9C}</c15:txfldGUID>
+                      <c15:txfldGUID>{D518DB96-D95F-42B8-9C47-7DEC8764D7DC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$139</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29171,7 +29237,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{957A40BA-4738-462E-8FBE-F106DC6FEECE}</c15:txfldGUID>
+                      <c15:txfldGUID>{C0293EA5-11F9-4DC2-B13E-86210C2537DB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$140</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29211,7 +29277,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4017B4AA-ED8D-4DF0-9967-47B2AF10189F}</c15:txfldGUID>
+                      <c15:txfldGUID>{8E084F51-5224-4A05-84A9-EE1D5A913B46}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$141</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29251,7 +29317,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{91407056-0B0E-45F5-BE50-B11BCA012D98}</c15:txfldGUID>
+                      <c15:txfldGUID>{30B164E3-250C-40D2-ADC5-F404C4A430C6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$142</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29291,7 +29357,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0338B522-C432-4006-8CF4-EE2BF8BA5A0B}</c15:txfldGUID>
+                      <c15:txfldGUID>{CEB4C0CC-4C73-4879-B9D4-06458D319618}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$143</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29331,7 +29397,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{22D14680-BAF2-47F4-9D33-439A206808F6}</c15:txfldGUID>
+                      <c15:txfldGUID>{E987C351-40D8-4841-BE66-C79059E064FC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$144</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29371,7 +29437,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{385138AE-5A17-48C3-BF79-8B5E69039693}</c15:txfldGUID>
+                      <c15:txfldGUID>{A03413BD-DE97-4B2B-81A3-BFC79EF075DE}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$145</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29411,7 +29477,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{561389AE-DEFE-40CB-BE97-11730585C75B}</c15:txfldGUID>
+                      <c15:txfldGUID>{BB5C0688-C68C-45D3-B13F-26E7A77C9BC0}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$146</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29451,7 +29517,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{65DCE590-D0B5-41A4-8175-3393FAB3E8AB}</c15:txfldGUID>
+                      <c15:txfldGUID>{085010C4-715E-41DD-8886-E1B92146C05C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$147</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29491,7 +29557,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{93428817-4382-491E-9E18-2434C3CBCD11}</c15:txfldGUID>
+                      <c15:txfldGUID>{DA586709-4BC3-420B-B93A-5412E66175BC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$148</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29531,7 +29597,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{562776F2-2AFC-4143-9F76-3FF98AE4FF64}</c15:txfldGUID>
+                      <c15:txfldGUID>{716102A5-4825-46FD-8761-CE321953293F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$149</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29571,7 +29637,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2CCE304E-6F94-4451-81C9-E31CCACB3845}</c15:txfldGUID>
+                      <c15:txfldGUID>{69A3AE2C-B6AE-44AF-A559-4BAAD7292031}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$150</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29611,7 +29677,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{03D73A70-3572-4BA2-8BA6-A7191F5A8207}</c15:txfldGUID>
+                      <c15:txfldGUID>{7362EAD4-D91D-4515-971E-E20CE5799DD2}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$151</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29651,7 +29717,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{11ACD940-79C5-48ED-A143-F79F03C88492}</c15:txfldGUID>
+                      <c15:txfldGUID>{7CFF98F3-4D3C-40A1-9C95-6D122C38610F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$152</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29691,7 +29757,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4A2B7DDB-7F18-4543-ACED-12AB0B9DC664}</c15:txfldGUID>
+                      <c15:txfldGUID>{F69FF7D6-DDB0-4762-8C09-1D384CB43289}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$153</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29731,7 +29797,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{29CCFD0E-26EB-4CAE-AB52-DAF5C5460A31}</c15:txfldGUID>
+                      <c15:txfldGUID>{83C121F7-E2BA-45C8-A73E-80C3DE7F8CB4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$154</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29771,7 +29837,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FCB4BDFE-D54D-4012-BAA7-C0C1323F1CC0}</c15:txfldGUID>
+                      <c15:txfldGUID>{B22D8F81-EDEF-4680-8880-4B175155F712}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$155</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29811,7 +29877,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3D5C98DE-7C64-4F77-90AB-0738BD35B5BD}</c15:txfldGUID>
+                      <c15:txfldGUID>{456BF99F-8775-4BFB-BF4A-800062F55067}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$156</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29851,7 +29917,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C369CC7D-37B4-43FE-BB35-DF7FF35ACB66}</c15:txfldGUID>
+                      <c15:txfldGUID>{DB4DE92C-90BF-4330-AFF0-4CBB5A0E1AEE}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$157</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29891,7 +29957,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8A30B2AF-416B-458B-AE89-7FEC9466FB25}</c15:txfldGUID>
+                      <c15:txfldGUID>{36F3576B-20D7-455F-92A9-D5FD851B2BFD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$158</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29931,7 +29997,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{99AA651B-4F25-460D-84F6-708D872E79B5}</c15:txfldGUID>
+                      <c15:txfldGUID>{8AF0AE4A-ED42-4E8A-92B1-9092285D0961}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$159</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -29971,7 +30037,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{66D44A69-0972-4036-9C73-7A40222498AC}</c15:txfldGUID>
+                      <c15:txfldGUID>{95FDE3A8-D2DC-4A6B-B6CD-1DC2A8ECD291}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$160</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30011,7 +30077,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{042035A2-EC62-4874-A6E0-0B7765DA8E1B}</c15:txfldGUID>
+                      <c15:txfldGUID>{91E3245A-098E-4103-9CFA-86D3672F717C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$161</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30051,7 +30117,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{44A58C72-6C5E-48F3-A866-C486FEA40957}</c15:txfldGUID>
+                      <c15:txfldGUID>{255679F2-6C36-4F1F-B77D-7FAD399BABF4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$162</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30091,7 +30157,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4500538E-D785-4413-89AB-1F7BE55D02F0}</c15:txfldGUID>
+                      <c15:txfldGUID>{CAA520A1-45BC-4A68-8134-D84115CA99F3}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$163</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30131,7 +30197,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{66C198F3-486B-4F0F-BE25-0D3130418C7C}</c15:txfldGUID>
+                      <c15:txfldGUID>{190A704E-E772-45E2-9177-13FB0CF12823}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$164</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30171,7 +30237,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{33DE0951-5998-4BBE-BF54-0BB11BA0480B}</c15:txfldGUID>
+                      <c15:txfldGUID>{C7E3D8B4-C2DB-4EA6-A24E-F1B4AC56483B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$165</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30211,7 +30277,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8FFF807A-B06F-475B-8B3E-371C8B752287}</c15:txfldGUID>
+                      <c15:txfldGUID>{8D725B00-05A6-4C76-BA51-187C246F0B89}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$166</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30251,7 +30317,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{46FA8136-3937-464B-A24F-5D54CB5D50BD}</c15:txfldGUID>
+                      <c15:txfldGUID>{EA37D231-DD4C-4B31-A8CB-FB4EE98A39E9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$167</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30291,7 +30357,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B22F46D9-FEEC-416D-B431-B04E70AD35E0}</c15:txfldGUID>
+                      <c15:txfldGUID>{B206A655-CF70-488D-ADD7-E6E32149A0DD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$168</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30331,7 +30397,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F117AD2F-0DBE-4389-BBA5-62256828C92D}</c15:txfldGUID>
+                      <c15:txfldGUID>{8B475812-EE19-4C50-B133-0256881981BA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$169</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30371,7 +30437,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{74A0352D-245D-4521-AC42-064764EEAC87}</c15:txfldGUID>
+                      <c15:txfldGUID>{CD7736F9-157C-40C0-852C-A48D765A9843}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$170</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -30423,10 +30489,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>('Bill Data'!$E$2:$E$46,'Bill Data'!$E$89:$E$253)</c:f>
+              <c:f>('Bill Data'!$E$2:$E$46,'Bill Data'!$E$89:$E$254)</c:f>
               <c:numCache>
                 <c:formatCode>0\°</c:formatCode>
-                <c:ptCount val="210"/>
+                <c:ptCount val="211"/>
                 <c:pt idx="0">
                   <c:v>69</c:v>
                 </c:pt>
@@ -31056,16 +31122,19 @@
                 </c:pt>
                 <c:pt idx="209">
                   <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('Bill Data'!$M$2:$M$46,'Bill Data'!$M$89:$M$253)</c:f>
+              <c:f>('Bill Data'!$M$2:$M$46,'Bill Data'!$M$89:$M$254)</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="210"/>
+                <c:ptCount val="211"/>
                 <c:pt idx="0">
                   <c:v>23.791666666666668</c:v>
                 </c:pt>
@@ -31695,6 +31764,9 @@
                 </c:pt>
                 <c:pt idx="209">
                   <c:v>28.741935483870968</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>24.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31746,7 +31818,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F7E1105B-3686-4275-A7E9-E28A4A1760AE}</c15:txfldGUID>
+                      <c15:txfldGUID>{46F1AFDE-126F-418D-88BA-7BB26C0B58FD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$47</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -31787,7 +31859,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EBAD4F68-0D62-4C47-8315-6140C84E6324}</c15:txfldGUID>
+                      <c15:txfldGUID>{4C8F5DA0-1C56-4BE1-822A-5E6B9DCE59CD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$48</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -31828,7 +31900,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3CE45098-E26B-4EAE-A94B-94778753054B}</c15:txfldGUID>
+                      <c15:txfldGUID>{33D6CC9D-2005-4109-8F8E-B2AB8F2DAD80}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$49</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -31869,7 +31941,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{80A34999-DA6D-45DF-BFEA-80EC51DA4023}</c15:txfldGUID>
+                      <c15:txfldGUID>{39DD2FD7-68BD-482B-B505-DE6821F6190D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$50</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -31910,7 +31982,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7DF866BE-1AF2-4713-9D3F-8E1AF94245A2}</c15:txfldGUID>
+                      <c15:txfldGUID>{14FA03E9-9AC0-435E-B182-829936525149}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$51</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -31951,7 +32023,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9E4881D6-9BA1-442C-B8A8-0EB8D1DA1CBB}</c15:txfldGUID>
+                      <c15:txfldGUID>{268B9104-86C1-4332-B410-624A8EB80D04}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$52</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -31992,7 +32064,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{01DF7D0E-90A8-45EF-B471-F88E195B8AB4}</c15:txfldGUID>
+                      <c15:txfldGUID>{2A6D5BE4-9EAC-4F0A-99B4-7F1DA8529B3B}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$53</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32033,7 +32105,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{109B613B-F576-4CB0-804C-88D27FA072E3}</c15:txfldGUID>
+                      <c15:txfldGUID>{6809D7DD-B1C7-42E6-9099-9CE0CC4FF1BD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$54</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32074,7 +32146,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{13E2D666-10DF-4F4F-AEB1-428F6188060F}</c15:txfldGUID>
+                      <c15:txfldGUID>{B72AA3BD-CDB0-4394-97F1-F0CB0C5016CD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$55</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32115,7 +32187,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2ACADF76-5ACF-4F6E-9870-26B5BB81532B}</c15:txfldGUID>
+                      <c15:txfldGUID>{7FC87B47-CD74-4D4B-8E24-E5BC7AA121BE}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$56</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32156,7 +32228,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4DD80C73-64D2-492E-8492-B9D3788AA7FB}</c15:txfldGUID>
+                      <c15:txfldGUID>{815978A5-E115-4B66-86F9-6153C31CECBD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$57</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32197,7 +32269,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CC28FF72-B28D-4891-8FF5-9C19E2E66B48}</c15:txfldGUID>
+                      <c15:txfldGUID>{A61A1911-C844-4730-9026-7D447AA38274}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$58</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32238,7 +32310,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EFF7786E-0253-44A3-A88F-D00309EE0E64}</c15:txfldGUID>
+                      <c15:txfldGUID>{67D826D2-6D1D-4753-8223-BD7B6E1391D9}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$59</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32279,7 +32351,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{76BB426D-7F9A-4182-8033-1E8841EC81DD}</c15:txfldGUID>
+                      <c15:txfldGUID>{D2D69414-056D-4BDB-87EC-DA5A5625F86F}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$60</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32320,7 +32392,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8469FA00-10E6-41F7-B60B-C2E78BFC6766}</c15:txfldGUID>
+                      <c15:txfldGUID>{0D672BB6-A5BF-4A7E-BF1D-AB3D160C38E6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$61</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32361,7 +32433,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{49C4F68A-2123-4E67-BEE5-5CAD85519E4A}</c15:txfldGUID>
+                      <c15:txfldGUID>{2DB7A2C7-3685-4090-A043-1E9E48A2657C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$62</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32402,7 +32474,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7BCBE3C8-8301-4DDC-8E08-830DA3EFA779}</c15:txfldGUID>
+                      <c15:txfldGUID>{80DDEFB0-2762-4E44-8F8D-515712DDF22A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$63</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32443,7 +32515,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CF7D4C04-7599-46D2-86A2-A3D75F247483}</c15:txfldGUID>
+                      <c15:txfldGUID>{B8F1B97B-4BAD-4DE4-8D26-876DF1CDDE7A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$64</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32484,7 +32556,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6B5C3431-BFDE-4D81-85BA-98845CAE9AC9}</c15:txfldGUID>
+                      <c15:txfldGUID>{30AEA02D-535E-4A4A-9E7A-7C578C3183DC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$65</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32525,7 +32597,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{56B3FB61-D5C8-4778-B3D9-3C0DE4FAAFA2}</c15:txfldGUID>
+                      <c15:txfldGUID>{CC81EFEE-1BD3-433F-9F35-BCA56FC9673C}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$66</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32566,7 +32638,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0FF9F19D-6CAC-484D-B242-A589EE1F9173}</c15:txfldGUID>
+                      <c15:txfldGUID>{29D87267-7563-4D43-BE15-A8050046451A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$67</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32607,7 +32679,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1653B4D1-11BD-4C44-9FE4-99CCCA772EA5}</c15:txfldGUID>
+                      <c15:txfldGUID>{9C847954-257F-4DD8-96BE-09BD9F5172ED}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$68</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32648,7 +32720,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D7B3EF9E-330A-479E-B5FD-93AD5163E449}</c15:txfldGUID>
+                      <c15:txfldGUID>{4ACD6680-9DE1-41A1-A66D-CBC8842491E4}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$69</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32689,7 +32761,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{509DAD34-37D8-4D0C-AC9B-02212520567E}</c15:txfldGUID>
+                      <c15:txfldGUID>{A864B0B6-777E-4CCB-94C7-62A4E47FC2CD}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32730,7 +32802,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F55C094B-DD43-40F2-BBD0-117B45259190}</c15:txfldGUID>
+                      <c15:txfldGUID>{2E4E7F35-F224-41AE-8756-C275A9D2FAA8}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$71</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32771,7 +32843,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AFB96BF6-3AC7-4C86-84CF-E7E3637CC4A0}</c15:txfldGUID>
+                      <c15:txfldGUID>{D088AECE-2369-4C95-B139-77E0A2912D81}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32812,7 +32884,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FA9CFA8C-8264-4EA1-A026-2F342D50877E}</c15:txfldGUID>
+                      <c15:txfldGUID>{2ED8FF0C-C335-4394-90E8-A3ABA57AE102}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$73</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32853,7 +32925,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{95FD731F-4F8A-4E42-B8D8-D3DCF238C601}</c15:txfldGUID>
+                      <c15:txfldGUID>{F4D70CFC-9DC2-42B9-A680-AE5D2CE2A08D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$74</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32894,7 +32966,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A3E058D3-16E4-45E8-88CB-9F3705AF99E2}</c15:txfldGUID>
+                      <c15:txfldGUID>{4FA6AE84-BE28-4AA3-80BD-24924CFD88BC}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$75</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32935,7 +33007,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{73BDFF86-2E10-43A7-A79D-28299EAA1816}</c15:txfldGUID>
+                      <c15:txfldGUID>{0EB1F184-3DA5-4BB0-976D-9080B282F39A}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$76</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -32976,7 +33048,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EBA1FDCE-7373-4FA1-9C13-F56ABAB2C9F9}</c15:txfldGUID>
+                      <c15:txfldGUID>{C66DABAB-5D6C-4601-8746-6E5758B09ACB}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$77</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33017,7 +33089,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3881ABA4-9A63-4588-ADA6-A36A4B0920D0}</c15:txfldGUID>
+                      <c15:txfldGUID>{E544AAED-A441-4C89-A68E-0BBEEDD18723}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$78</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33058,7 +33130,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EE078D16-EA11-482C-A568-7BD2CB69203D}</c15:txfldGUID>
+                      <c15:txfldGUID>{F2B239C5-D65A-496C-B966-5A3DD03B71BA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$79</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33099,7 +33171,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{165A7F21-0ECA-4D33-93E7-3D695840080F}</c15:txfldGUID>
+                      <c15:txfldGUID>{59A0DAF7-E3D9-4D6A-8FDA-E7EBCA0C0C70}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$80</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33140,7 +33212,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{57F7DF54-695D-472E-B3F8-7B6E0C82BA06}</c15:txfldGUID>
+                      <c15:txfldGUID>{9DDBF383-2272-457B-83B4-3BA79DB706BA}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$81</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33181,7 +33253,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{74708A57-0F5C-41BC-84EF-94F7037F82EF}</c15:txfldGUID>
+                      <c15:txfldGUID>{4853252C-A501-4191-BC34-5CDAB1FD2374}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$82</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33222,7 +33294,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CA166C3C-3E5C-4E7D-ABDA-A93DDBE3A221}</c15:txfldGUID>
+                      <c15:txfldGUID>{7698259E-FA05-43FA-9941-BF283C7B1FE6}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$83</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33263,7 +33335,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1783BF55-1115-4B9E-8CF8-39F4A2E4E349}</c15:txfldGUID>
+                      <c15:txfldGUID>{B5732EF6-3DA4-4562-BEA6-013E4D4C49F5}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$84</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33304,7 +33376,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{282DDE24-8B2B-4FB6-AD9A-B2E66E93B115}</c15:txfldGUID>
+                      <c15:txfldGUID>{78041243-AB5B-49AA-917C-E05CBC28E913}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$85</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33345,7 +33417,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DA62DC9D-0F45-4D43-809A-09248FB87118}</c15:txfldGUID>
+                      <c15:txfldGUID>{E57A70AA-9A20-440E-BD45-188022A2866D}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$86</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33392,7 +33464,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{196C74A9-19C2-4B68-A401-4A3DCB685B1F}</c15:txfldGUID>
+                      <c15:txfldGUID>{47D08EE0-6F4B-43C9-8C6F-F5D0638D2AF5}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$87</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33433,7 +33505,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F59C6E3D-0551-4D72-9E78-64391449EB68}</c15:txfldGUID>
+                      <c15:txfldGUID>{CF83D577-CADA-4F75-AAEF-5354C2BD3966}</c15:txfldGUID>
                       <c15:f>'Bill Data'!$B$88</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -33930,10 +34002,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Bill Data'!$E$2:$E$253</c:f>
+              <c:f>'Bill Data'!$E$2:$E$254</c:f>
               <c:numCache>
                 <c:formatCode>0\°</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>69</c:v>
                 </c:pt>
@@ -34689,16 +34761,19 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Bill Data'!$F$2:$F$253</c:f>
+              <c:f>'Bill Data'!$F$2:$F$254</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="252"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>43.7</c:v>
                 </c:pt>
@@ -35454,6 +35529,9 @@
                 </c:pt>
                 <c:pt idx="251">
                   <c:v>150.73000000000002</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>125.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -37250,11 +37328,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U253"/>
+  <dimension ref="A1:U254"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R255" sqref="R255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -43402,11 +43480,11 @@
         <v>40091</v>
       </c>
       <c r="B98" s="12" t="str">
-        <f t="shared" ref="B98:B253" si="19">MONTH(A98) &amp; "/" &amp; RIGHT(YEAR(A98),2)</f>
+        <f t="shared" ref="B98:B254" si="19">MONTH(A98) &amp; "/" &amp; RIGHT(YEAR(A98),2)</f>
         <v>10/09</v>
       </c>
       <c r="C98">
-        <f t="shared" ref="C98:C253" si="20">MONTH(A98)</f>
+        <f t="shared" ref="C98:C254" si="20">MONTH(A98)</f>
         <v>10</v>
       </c>
       <c r="D98">
@@ -43436,7 +43514,7 @@
         <v>6.7902298850574708E-2</v>
       </c>
       <c r="M98" s="3">
-        <f t="shared" ref="M98:M253" si="22">K98/D98</f>
+        <f t="shared" ref="M98:M254" si="22">K98/D98</f>
         <v>21.75</v>
       </c>
       <c r="N98" s="7">
@@ -45432,7 +45510,7 @@
         <v>69</v>
       </c>
       <c r="F130" s="4">
-        <f t="shared" ref="F130:F161" si="24">G130+N130</f>
+        <f t="shared" ref="F130:F160" si="24">G130+N130</f>
         <v>71.150000000000006</v>
       </c>
       <c r="G130" s="5">
@@ -48443,7 +48521,7 @@
         <v>57</v>
       </c>
       <c r="F177" s="4">
-        <f t="shared" ref="F177:F253" si="28">G177+N177</f>
+        <f t="shared" ref="F177:F254" si="28">G177+N177</f>
         <v>64.66</v>
       </c>
       <c r="G177" s="5">
@@ -49535,7 +49613,7 @@
         <v>549</v>
       </c>
       <c r="L194" s="9">
-        <f t="shared" ref="L194:L253" si="29">(G194-H194)/K194</f>
+        <f t="shared" ref="L194:L254" si="29">(G194-H194)/K194</f>
         <v>9.4663023679417119E-2</v>
       </c>
       <c r="M194" s="3">
@@ -49555,11 +49633,11 @@
         <v>7</v>
       </c>
       <c r="S194" s="10">
-        <f t="shared" ref="S194:S257" si="30">(N194-O194)/R194</f>
+        <f t="shared" ref="S194:S254" si="30">(N194-O194)/R194</f>
         <v>0.9457142857142854</v>
       </c>
       <c r="T194" s="3">
-        <f t="shared" ref="T194:T253" si="31">R194/D194</f>
+        <f t="shared" ref="T194:T254" si="31">R194/D194</f>
         <v>0.2413793103448276</v>
       </c>
     </row>
@@ -50857,7 +50935,7 @@
         <v>80.66</v>
       </c>
       <c r="H215" s="8">
-        <f t="shared" ref="H215:H253" si="32">D215*J215</f>
+        <f t="shared" ref="H215:H254" si="32">D215*J215</f>
         <v>14.4</v>
       </c>
       <c r="J215" s="8">
@@ -50943,7 +51021,7 @@
         <v>25.78</v>
       </c>
       <c r="O216" s="8">
-        <f t="shared" ref="O216:O253" si="33">Q216*D216</f>
+        <f t="shared" ref="O216:O254" si="33">Q216*D216</f>
         <v>18.850000000000001</v>
       </c>
       <c r="Q216" s="8">
@@ -53364,6 +53442,71 @@
       <c r="T253" s="3">
         <f t="shared" si="31"/>
         <v>0.25806451612903225</v>
+      </c>
+    </row>
+    <row r="254" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>44853</v>
+      </c>
+      <c r="B254" s="11" t="str">
+        <f t="shared" si="19"/>
+        <v>10/22</v>
+      </c>
+      <c r="C254">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="D254">
+        <v>30</v>
+      </c>
+      <c r="E254" s="2">
+        <v>76</v>
+      </c>
+      <c r="F254" s="4">
+        <f t="shared" si="28"/>
+        <v>125.37</v>
+      </c>
+      <c r="G254" s="5">
+        <v>96.33</v>
+      </c>
+      <c r="H254" s="8">
+        <f t="shared" si="32"/>
+        <v>13.5</v>
+      </c>
+      <c r="J254" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="K254">
+        <v>738</v>
+      </c>
+      <c r="L254" s="9">
+        <f t="shared" si="29"/>
+        <v>0.11223577235772357</v>
+      </c>
+      <c r="M254" s="3">
+        <f t="shared" si="22"/>
+        <v>24.6</v>
+      </c>
+      <c r="N254" s="7">
+        <v>29.04</v>
+      </c>
+      <c r="O254" s="8">
+        <f t="shared" si="33"/>
+        <v>19.5</v>
+      </c>
+      <c r="Q254" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="R254">
+        <v>6</v>
+      </c>
+      <c r="S254" s="10">
+        <f t="shared" si="30"/>
+        <v>1.5899999999999999</v>
+      </c>
+      <c r="T254" s="3">
+        <f t="shared" si="31"/>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>